<commit_message>
Added dictionaries and looping through file
</commit_message>
<xml_diff>
--- a/Logs/Keys_changed.xlsx
+++ b/Logs/Keys_changed.xlsx
@@ -644,7 +644,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:G2049"/>
+  <dimension ref="A1:G2050"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A1954" activePane="bottomLeft" state="frozen"/>
@@ -58793,29 +58793,66 @@
       </c>
     </row>
     <row r="2049">
-      <c r="A2049" t="inlineStr">
+      <c r="A2049" s="0" t="inlineStr">
         <is>
           <t>20.07.2020</t>
         </is>
       </c>
-      <c r="B2049" t="inlineStr">
-        <is>
-          <t>forms</t>
-        </is>
-      </c>
-      <c r="C2049" t="inlineStr">
+      <c r="B2049" s="0" t="inlineStr">
+        <is>
+          <t>forms</t>
+        </is>
+      </c>
+      <c r="C2049" s="0" t="inlineStr">
         <is>
           <t>app.invoice_group.save_alert_text</t>
         </is>
       </c>
-      <c r="D2049" t="inlineStr">
+      <c r="D2049" s="0" t="inlineStr">
         <is>
           <t>Grupa fakturowa będzie zapisana i powiadomienie zostanie wysłane do płatnika.</t>
         </is>
       </c>
-      <c r="E2049" t="inlineStr">
+      <c r="E2049" s="0" t="inlineStr">
         <is>
           <t>Invoice group will be saved and notification will be sent to payer.</t>
+        </is>
+      </c>
+    </row>
+    <row r="2050">
+      <c r="A2050" t="inlineStr">
+        <is>
+          <t>21.07.2020</t>
+        </is>
+      </c>
+      <c r="B2050" t="inlineStr">
+        <is>
+          <t>messages</t>
+        </is>
+      </c>
+      <c r="C2050" t="inlineStr">
+        <is>
+          <t>app.order_reports_invoice.currency</t>
+        </is>
+      </c>
+      <c r="D2050" t="inlineStr">
+        <is>
+          <t>Waluta</t>
+        </is>
+      </c>
+      <c r="E2050" t="inlineStr">
+        <is>
+          <t>Currency</t>
+        </is>
+      </c>
+      <c r="F2050" t="inlineStr">
+        <is>
+          <t>Waluta z cennika</t>
+        </is>
+      </c>
+      <c r="G2050" t="inlineStr">
+        <is>
+          <t>Currency from pricing</t>
         </is>
       </c>
     </row>

</xml_diff>